<commit_message>
change data of excel file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\django files\se project\Seman-Dormitory-Project-main\Seman-Dormitory-Project-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D2FCF-8A4C-44E8-9138-5431C323D798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DA8690-9078-442C-A7A1-CC07F2F94F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59,10 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,174 +341,118 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>8687982933</v>
+      <c r="A1">
+        <v>1111111111</v>
       </c>
       <c r="B1">
-        <v>9811126100</v>
+        <v>9811126101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>7852859496</v>
+      <c r="A2">
+        <v>2222222222</v>
       </c>
       <c r="B2">
-        <v>9811126101</v>
+        <v>9811126034</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>3113625556</v>
+      <c r="A3">
+        <v>3333333333</v>
       </c>
       <c r="B3">
-        <v>9811126102</v>
+        <v>9811126041</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3892778558</v>
+      <c r="A4">
+        <v>1234567890</v>
       </c>
       <c r="B4">
-        <v>9811126103</v>
+        <v>9811126033</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2957318733</v>
+      <c r="A5">
+        <v>2345678910</v>
       </c>
       <c r="B5">
-        <v>9811126108</v>
+        <v>9811126072</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>1219996157</v>
+      <c r="A6">
+        <v>3456789120</v>
       </c>
       <c r="B6">
-        <v>9911148059</v>
+        <v>9811126087</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>7469659536</v>
-      </c>
-      <c r="B7">
-        <v>9711169012</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>3017299651</v>
-      </c>
-      <c r="B8">
-        <v>9812126030</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>2626926434</v>
-      </c>
-      <c r="B9">
-        <v>9911126082</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>8443947470</v>
-      </c>
-      <c r="B10">
-        <v>9811126072</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>5072337383</v>
-      </c>
-      <c r="B11">
-        <v>9811126041</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>5248574579</v>
-      </c>
-      <c r="B12">
-        <v>9811126033</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>7595727863</v>
-      </c>
-      <c r="B13">
-        <v>9811126087</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>5927395155</v>
-      </c>
-      <c r="B14">
-        <v>9811126034</v>
-      </c>
+      <c r="A14"/>
+      <c r="B14"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>1896137881</v>
-      </c>
-      <c r="B15">
-        <v>9811126009</v>
-      </c>
+      <c r="A15"/>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>1966488912</v>
-      </c>
-      <c r="B16">
-        <v>9611126385</v>
-      </c>
+      <c r="A16"/>
+      <c r="B16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>2269448626</v>
-      </c>
-      <c r="B17">
-        <v>9911126039</v>
-      </c>
+      <c r="A17"/>
+      <c r="B17"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>6143691916</v>
-      </c>
-      <c r="B18">
-        <v>9911127089</v>
-      </c>
+      <c r="A18"/>
+      <c r="B18"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>7325421842</v>
-      </c>
-      <c r="B19">
-        <v>9811126049</v>
-      </c>
+      <c r="A19"/>
+      <c r="B19"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>3632981434</v>
-      </c>
-      <c r="B20">
-        <v>9911126076</v>
-      </c>
+      <c r="A20"/>
+      <c r="B20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>